<commit_message>
Actualizar plantillas Excel y API de importación para coherencia con formulario
- Agregar columna SKU al template de productos y su mapeo en la API
- Renombrar columnas: status→estado, tags→etiquetas, tamaño_nominal→medida_nominal, tamaño_real→medida_real, bind_code→id_bind
- Renombrar status→estado en template de categorías
- Mantener nombres anteriores como alias en la API para compatibilidad

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/templates/productos-template.xlsx
+++ b/public/templates/productos-template.xlsx
@@ -397,344 +397,353 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ3"/>
+  <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>sku</v>
+      </c>
+      <c r="B1" t="str">
         <v>nombre</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
         <v>nombre_en</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>descripcion</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>descripcion_en</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>precio</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>moneda</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>precio_usd</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>categoria</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>categoria_en</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>categoria_filtro</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>stock</v>
       </c>
-      <c r="L1" t="str">
-        <v>status</v>
-      </c>
       <c r="M1" t="str">
-        <v>tags</v>
+        <v>estado</v>
       </c>
       <c r="N1" t="str">
-        <v>tamaño_nominal</v>
+        <v>etiquetas</v>
       </c>
       <c r="O1" t="str">
-        <v>tamaño_real</v>
+        <v>medida_nominal</v>
       </c>
       <c r="P1" t="str">
+        <v>medida_real</v>
+      </c>
+      <c r="Q1" t="str">
         <v>dimensiones</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="R1" t="str">
         <v>peso</v>
       </c>
-      <c r="R1" t="str">
+      <c r="S1" t="str">
         <v>material</v>
       </c>
-      <c r="S1" t="str">
+      <c r="T1" t="str">
         <v>garantia</v>
       </c>
-      <c r="T1" t="str">
+      <c r="U1" t="str">
         <v>bind_id</v>
       </c>
-      <c r="U1" t="str">
-        <v>bind_code</v>
-      </c>
       <c r="V1" t="str">
+        <v>id_bind</v>
+      </c>
+      <c r="W1" t="str">
         <v>eficiencia</v>
       </c>
-      <c r="W1" t="str">
+      <c r="X1" t="str">
         <v>eficiencia_en</v>
       </c>
-      <c r="X1" t="str">
+      <c r="Y1" t="str">
         <v>clase_eficiencia</v>
       </c>
-      <c r="Y1" t="str">
+      <c r="Z1" t="str">
         <v>caracteristicas</v>
       </c>
-      <c r="Z1" t="str">
+      <c r="AA1" t="str">
         <v>caracteristicas_en</v>
       </c>
-      <c r="AA1" t="str">
+      <c r="AB1" t="str">
         <v>material_marco</v>
       </c>
-      <c r="AB1" t="str">
+      <c r="AC1" t="str">
         <v>temperatura_maxima</v>
       </c>
-      <c r="AC1" t="str">
+      <c r="AD1" t="str">
         <v>instalacion_tipica</v>
       </c>
-      <c r="AD1" t="str">
+      <c r="AE1" t="str">
         <v>instalacion_tipica_en</v>
       </c>
-      <c r="AE1" t="str">
+      <c r="AF1" t="str">
         <v>aplicaciones</v>
       </c>
-      <c r="AF1" t="str">
+      <c r="AG1" t="str">
         <v>aplicaciones_en</v>
       </c>
-      <c r="AG1" t="str">
+      <c r="AH1" t="str">
         <v>beneficios</v>
       </c>
-      <c r="AH1" t="str">
+      <c r="AI1" t="str">
         <v>beneficios_en</v>
       </c>
-      <c r="AI1" t="str">
+      <c r="AJ1" t="str">
         <v>imagen_principal</v>
       </c>
-      <c r="AJ1" t="str">
+      <c r="AK1" t="str">
         <v>imagenes_carrusel</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>SF-HEPA-H13-2424</v>
+      </c>
+      <c r="B2" t="str">
         <v>Filtro HEPA H13</v>
       </c>
-      <c r="B2" t="str">
+      <c r="C2" t="str">
         <v>HEPA Filter H13</v>
       </c>
-      <c r="C2" t="str">
+      <c r="D2" t="str">
         <v>Filtro HEPA de alta eficiencia para cuartos limpios</v>
       </c>
-      <c r="D2" t="str">
+      <c r="E2" t="str">
         <v>High efficiency HEPA filter for cleanrooms</v>
       </c>
-      <c r="E2" t="str">
+      <c r="F2" t="str">
         <v>1500.00</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" t="str">
         <v>MXN</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <v>75.00</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <v>Filtros de Aire</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" t="str">
         <v>Air Filters</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" t="str">
         <v>HEPA</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L2" t="str">
         <v>100</v>
       </c>
-      <c r="L2" t="str">
+      <c r="M2" t="str">
         <v>active</v>
       </c>
-      <c r="M2" t="str">
+      <c r="N2" t="str">
         <v>hepa, filtro, cuarto limpio</v>
-      </c>
-      <c r="N2" t="str">
-        <v>24x24x11.5</v>
       </c>
       <c r="O2" t="str">
         <v>24x24x11.5</v>
       </c>
       <c r="P2" t="str">
+        <v>24x24x11.5</v>
+      </c>
+      <c r="Q2" t="str">
         <v>610x610x292mm</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="R2" t="str">
         <v>5kg</v>
       </c>
-      <c r="R2" t="str">
+      <c r="S2" t="str">
         <v>Aluminio</v>
       </c>
-      <c r="S2" t="str">
+      <c r="T2" t="str">
         <v>1 año</v>
       </c>
-      <c r="T2" t="str">
+      <c r="U2" t="str">
         <v/>
       </c>
-      <c r="U2" t="str">
+      <c r="V2" t="str">
         <v>HEPA-24-24-H13</v>
       </c>
-      <c r="V2" t="str">
+      <c r="W2" t="str">
         <v>99.97% a 0.3µm</v>
       </c>
-      <c r="W2" t="str">
+      <c r="X2" t="str">
         <v>99.97% at 0.3µm</v>
       </c>
-      <c r="X2" t="str">
+      <c r="Y2" t="str">
         <v>H13</v>
       </c>
-      <c r="Y2" t="str">
+      <c r="Z2" t="str">
         <v>Marco de aluminio, sellado con goma</v>
       </c>
-      <c r="Z2" t="str">
+      <c r="AA2" t="str">
         <v>Aluminum frame, rubber sealed</v>
       </c>
-      <c r="AA2" t="str">
+      <c r="AB2" t="str">
         <v>Aluminio</v>
       </c>
-      <c r="AB2" t="str">
+      <c r="AC2" t="str">
         <v>70°C</v>
       </c>
-      <c r="AC2" t="str">
+      <c r="AD2" t="str">
         <v>Sistema de filtración de aire</v>
       </c>
-      <c r="AD2" t="str">
+      <c r="AE2" t="str">
         <v>Air filtration system</v>
       </c>
-      <c r="AE2" t="str">
+      <c r="AF2" t="str">
         <v>Cuartos limpios, hospitales</v>
       </c>
-      <c r="AF2" t="str">
+      <c r="AG2" t="str">
         <v>Cleanrooms, hospitals</v>
       </c>
-      <c r="AG2" t="str">
+      <c r="AH2" t="str">
         <v>Alta eficiencia, bajo consumo</v>
       </c>
-      <c r="AH2" t="str">
+      <c r="AI2" t="str">
         <v>High efficiency, low consumption</v>
       </c>
-      <c r="AI2" t="str">
+      <c r="AJ2" t="str">
         <v>https://ejemplo.com/imagen-principal.jpg</v>
       </c>
-      <c r="AJ2" t="str">
+      <c r="AK2" t="str">
         <v>https://ejemplo.com/imagen1.jpg,https://ejemplo.com/imagen2.jpg</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>SF-PRE-G4-2020</v>
+      </c>
+      <c r="B3" t="str">
         <v>Filtro Prefiltro G4</v>
       </c>
-      <c r="B3" t="str">
+      <c r="C3" t="str">
         <v>Pre-filter G4</v>
       </c>
-      <c r="C3" t="str">
+      <c r="D3" t="str">
         <v>Prefiltro de baja eficiencia para sistemas de ventilación</v>
       </c>
-      <c r="D3" t="str">
+      <c r="E3" t="str">
         <v>Low efficiency pre-filter for ventilation systems</v>
       </c>
-      <c r="E3" t="str">
+      <c r="F3" t="str">
         <v>250.00</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" t="str">
         <v>MXN</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <v>12.50</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <v>Filtros de Aire</v>
       </c>
-      <c r="I3" t="str">
+      <c r="J3" t="str">
         <v>Air Filters</v>
       </c>
-      <c r="J3" t="str">
+      <c r="K3" t="str">
         <v>Prefiltros</v>
       </c>
-      <c r="K3" t="str">
+      <c r="L3" t="str">
         <v>50</v>
       </c>
-      <c r="L3" t="str">
+      <c r="M3" t="str">
         <v>inactive</v>
       </c>
-      <c r="M3" t="str">
+      <c r="N3" t="str">
         <v>prefiltro, ventilacion</v>
-      </c>
-      <c r="N3" t="str">
-        <v>20x20x2</v>
       </c>
       <c r="O3" t="str">
         <v>20x20x2</v>
       </c>
       <c r="P3" t="str">
+        <v>20x20x2</v>
+      </c>
+      <c r="Q3" t="str">
         <v>500x500x50mm</v>
       </c>
-      <c r="Q3" t="str">
+      <c r="R3" t="str">
         <v>1.5kg</v>
       </c>
-      <c r="R3" t="str">
+      <c r="S3" t="str">
         <v>Cartón</v>
       </c>
-      <c r="S3" t="str">
+      <c r="T3" t="str">
         <v>6 meses</v>
       </c>
-      <c r="T3" t="str">
+      <c r="U3" t="str">
         <v/>
       </c>
-      <c r="U3" t="str">
+      <c r="V3" t="str">
         <v>PRE-G4-20-20</v>
       </c>
-      <c r="V3" t="str">
+      <c r="W3" t="str">
         <v>35% a 0.3µm</v>
       </c>
-      <c r="W3" t="str">
+      <c r="X3" t="str">
         <v>35% at 0.3µm</v>
       </c>
-      <c r="X3" t="str">
+      <c r="Y3" t="str">
         <v>G4</v>
       </c>
-      <c r="Y3" t="str">
+      <c r="Z3" t="str">
         <v>Marco de cartón, fácil instalación</v>
       </c>
-      <c r="Z3" t="str">
+      <c r="AA3" t="str">
         <v>Cardboard frame, easy installation</v>
       </c>
-      <c r="AA3" t="str">
+      <c r="AB3" t="str">
         <v>Cartón</v>
       </c>
-      <c r="AB3" t="str">
+      <c r="AC3" t="str">
         <v>60°C</v>
       </c>
-      <c r="AC3" t="str">
+      <c r="AD3" t="str">
         <v>Sistemas de ventilación general</v>
       </c>
-      <c r="AD3" t="str">
+      <c r="AE3" t="str">
         <v>General ventilation systems</v>
       </c>
-      <c r="AE3" t="str">
+      <c r="AF3" t="str">
         <v>Oficinas, comercios</v>
       </c>
-      <c r="AF3" t="str">
+      <c r="AG3" t="str">
         <v>Offices, commercial</v>
       </c>
-      <c r="AG3" t="str">
+      <c r="AH3" t="str">
         <v>Bajo costo, fácil mantenimiento</v>
       </c>
-      <c r="AH3" t="str">
+      <c r="AI3" t="str">
         <v>Low cost, easy maintenance</v>
       </c>
-      <c r="AI3" t="str">
+      <c r="AJ3" t="str">
         <v/>
       </c>
-      <c r="AJ3" t="str">
+      <c r="AK3" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AJ3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AK3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregar campo 'Código de producto' a productos: plantilla Excel, importación y servicios
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/public/templates/productos-template.xlsx
+++ b/public/templates/productos-template.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK3"/>
+  <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -470,48 +470,51 @@
         <v>id_bind</v>
       </c>
       <c r="W1" t="str">
+        <v>codigo_de_producto</v>
+      </c>
+      <c r="X1" t="str">
         <v>eficiencia</v>
       </c>
-      <c r="X1" t="str">
+      <c r="Y1" t="str">
         <v>eficiencia_en</v>
       </c>
-      <c r="Y1" t="str">
+      <c r="Z1" t="str">
         <v>clase_eficiencia</v>
       </c>
-      <c r="Z1" t="str">
+      <c r="AA1" t="str">
         <v>caracteristicas</v>
       </c>
-      <c r="AA1" t="str">
+      <c r="AB1" t="str">
         <v>caracteristicas_en</v>
       </c>
-      <c r="AB1" t="str">
+      <c r="AC1" t="str">
         <v>material_marco</v>
       </c>
-      <c r="AC1" t="str">
+      <c r="AD1" t="str">
         <v>temperatura_maxima</v>
       </c>
-      <c r="AD1" t="str">
+      <c r="AE1" t="str">
         <v>instalacion_tipica</v>
       </c>
-      <c r="AE1" t="str">
+      <c r="AF1" t="str">
         <v>instalacion_tipica_en</v>
       </c>
-      <c r="AF1" t="str">
+      <c r="AG1" t="str">
         <v>aplicaciones</v>
       </c>
-      <c r="AG1" t="str">
+      <c r="AH1" t="str">
         <v>aplicaciones_en</v>
       </c>
-      <c r="AH1" t="str">
+      <c r="AI1" t="str">
         <v>beneficios</v>
       </c>
-      <c r="AI1" t="str">
+      <c r="AJ1" t="str">
         <v>beneficios_en</v>
       </c>
-      <c r="AJ1" t="str">
+      <c r="AK1" t="str">
         <v>imagen_principal</v>
       </c>
-      <c r="AK1" t="str">
+      <c r="AL1" t="str">
         <v>imagenes_carrusel</v>
       </c>
     </row>
@@ -583,48 +586,51 @@
         <v>HEPA-24-24-H13</v>
       </c>
       <c r="W2" t="str">
+        <v>SF-HEPA-H13-001</v>
+      </c>
+      <c r="X2" t="str">
         <v>99.97% a 0.3µm</v>
       </c>
-      <c r="X2" t="str">
+      <c r="Y2" t="str">
         <v>99.97% at 0.3µm</v>
       </c>
-      <c r="Y2" t="str">
+      <c r="Z2" t="str">
         <v>H13</v>
       </c>
-      <c r="Z2" t="str">
+      <c r="AA2" t="str">
         <v>Marco de aluminio, sellado con goma</v>
       </c>
-      <c r="AA2" t="str">
+      <c r="AB2" t="str">
         <v>Aluminum frame, rubber sealed</v>
       </c>
-      <c r="AB2" t="str">
+      <c r="AC2" t="str">
         <v>Aluminio</v>
       </c>
-      <c r="AC2" t="str">
+      <c r="AD2" t="str">
         <v>70°C</v>
       </c>
-      <c r="AD2" t="str">
+      <c r="AE2" t="str">
         <v>Sistema de filtración de aire</v>
       </c>
-      <c r="AE2" t="str">
+      <c r="AF2" t="str">
         <v>Air filtration system</v>
       </c>
-      <c r="AF2" t="str">
+      <c r="AG2" t="str">
         <v>Cuartos limpios, hospitales</v>
       </c>
-      <c r="AG2" t="str">
+      <c r="AH2" t="str">
         <v>Cleanrooms, hospitals</v>
       </c>
-      <c r="AH2" t="str">
+      <c r="AI2" t="str">
         <v>Alta eficiencia, bajo consumo</v>
       </c>
-      <c r="AI2" t="str">
+      <c r="AJ2" t="str">
         <v>High efficiency, low consumption</v>
       </c>
-      <c r="AJ2" t="str">
+      <c r="AK2" t="str">
         <v>https://ejemplo.com/imagen-principal.jpg</v>
       </c>
-      <c r="AK2" t="str">
+      <c r="AL2" t="str">
         <v>https://ejemplo.com/imagen1.jpg,https://ejemplo.com/imagen2.jpg</v>
       </c>
     </row>
@@ -696,54 +702,57 @@
         <v>PRE-G4-20-20</v>
       </c>
       <c r="W3" t="str">
+        <v>SF-PRE-G4-001</v>
+      </c>
+      <c r="X3" t="str">
         <v>35% a 0.3µm</v>
       </c>
-      <c r="X3" t="str">
+      <c r="Y3" t="str">
         <v>35% at 0.3µm</v>
       </c>
-      <c r="Y3" t="str">
+      <c r="Z3" t="str">
         <v>G4</v>
       </c>
-      <c r="Z3" t="str">
+      <c r="AA3" t="str">
         <v>Marco de cartón, fácil instalación</v>
       </c>
-      <c r="AA3" t="str">
+      <c r="AB3" t="str">
         <v>Cardboard frame, easy installation</v>
       </c>
-      <c r="AB3" t="str">
+      <c r="AC3" t="str">
         <v>Cartón</v>
       </c>
-      <c r="AC3" t="str">
+      <c r="AD3" t="str">
         <v>60°C</v>
       </c>
-      <c r="AD3" t="str">
+      <c r="AE3" t="str">
         <v>Sistemas de ventilación general</v>
       </c>
-      <c r="AE3" t="str">
+      <c r="AF3" t="str">
         <v>General ventilation systems</v>
       </c>
-      <c r="AF3" t="str">
+      <c r="AG3" t="str">
         <v>Oficinas, comercios</v>
       </c>
-      <c r="AG3" t="str">
+      <c r="AH3" t="str">
         <v>Offices, commercial</v>
       </c>
-      <c r="AH3" t="str">
+      <c r="AI3" t="str">
         <v>Bajo costo, fácil mantenimiento</v>
       </c>
-      <c r="AI3" t="str">
+      <c r="AJ3" t="str">
         <v>Low cost, easy maintenance</v>
       </c>
-      <c r="AJ3" t="str">
+      <c r="AK3" t="str">
         <v/>
       </c>
-      <c r="AK3" t="str">
+      <c r="AL3" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AK3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AL3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregar campo 'Flujo de aire' a variantes: BD, admin, frontend y plantilla Excel
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/public/templates/productos-template.xlsx
+++ b/public/templates/productos-template.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL3"/>
+  <dimension ref="A1:AM3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -473,48 +473,51 @@
         <v>codigo_de_producto</v>
       </c>
       <c r="X1" t="str">
+        <v>flujo_aire</v>
+      </c>
+      <c r="Y1" t="str">
         <v>eficiencia</v>
       </c>
-      <c r="Y1" t="str">
+      <c r="Z1" t="str">
         <v>eficiencia_en</v>
       </c>
-      <c r="Z1" t="str">
+      <c r="AA1" t="str">
         <v>clase_eficiencia</v>
       </c>
-      <c r="AA1" t="str">
+      <c r="AB1" t="str">
         <v>caracteristicas</v>
       </c>
-      <c r="AB1" t="str">
+      <c r="AC1" t="str">
         <v>caracteristicas_en</v>
       </c>
-      <c r="AC1" t="str">
+      <c r="AD1" t="str">
         <v>material_marco</v>
       </c>
-      <c r="AD1" t="str">
+      <c r="AE1" t="str">
         <v>temperatura_maxima</v>
       </c>
-      <c r="AE1" t="str">
+      <c r="AF1" t="str">
         <v>instalacion_tipica</v>
       </c>
-      <c r="AF1" t="str">
+      <c r="AG1" t="str">
         <v>instalacion_tipica_en</v>
       </c>
-      <c r="AG1" t="str">
+      <c r="AH1" t="str">
         <v>aplicaciones</v>
       </c>
-      <c r="AH1" t="str">
+      <c r="AI1" t="str">
         <v>aplicaciones_en</v>
       </c>
-      <c r="AI1" t="str">
+      <c r="AJ1" t="str">
         <v>beneficios</v>
       </c>
-      <c r="AJ1" t="str">
+      <c r="AK1" t="str">
         <v>beneficios_en</v>
       </c>
-      <c r="AK1" t="str">
+      <c r="AL1" t="str">
         <v>imagen_principal</v>
       </c>
-      <c r="AL1" t="str">
+      <c r="AM1" t="str">
         <v>imagenes_carrusel</v>
       </c>
     </row>
@@ -752,7 +755,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AL3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AM3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>